<commit_message>
Added json generator for invalid forms
</commit_message>
<xml_diff>
--- a/test_back/test_forms/difficult_shapes_with_empty_spaces/TestCases lego_assembly_backend.xlsx
+++ b/test_back/test_forms/difficult_shapes_with_empty_spaces/TestCases lego_assembly_backend.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabitzu\Desktop\materii_facultate\Inteligenta_Artificiala\teste forme_goale\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sapuscasitei\Desktop\lego_backend\lego-assembly-back\test_back\test_forms\difficult_shapes_with_empty_spaces\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9285"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9288"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Questions" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -877,24 +878,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.46484375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="13.53125" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="20.46484375" customWidth="1"/>
-    <col min="5" max="5" width="22.19921875" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1"/>
+    <col min="5" max="5" width="22.21875" customWidth="1"/>
     <col min="6" max="6" width="32" customWidth="1"/>
-    <col min="7" max="7" width="19.86328125" customWidth="1"/>
-    <col min="8" max="8" width="18.53125" customWidth="1"/>
-    <col min="9" max="9" width="11.46484375" customWidth="1"/>
+    <col min="7" max="7" width="19.88671875" customWidth="1"/>
+    <col min="8" max="8" width="18.5546875" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -902,7 +903,7 @@
         <v>43171</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -910,7 +911,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>20</v>
       </c>
@@ -939,7 +940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="11"/>
@@ -955,7 +956,7 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>1</v>
       </c>
@@ -975,7 +976,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>2</v>
       </c>
@@ -995,7 +996,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>3</v>
       </c>
@@ -1015,7 +1016,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>4</v>
       </c>
@@ -1035,7 +1036,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>5</v>
       </c>
@@ -1052,7 +1053,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>6</v>
       </c>
@@ -1069,7 +1070,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>7</v>
       </c>
@@ -1086,7 +1087,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>8</v>
       </c>
@@ -1103,7 +1104,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>9</v>
       </c>
@@ -1120,7 +1121,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>10</v>
       </c>
@@ -1151,23 +1152,23 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.796875" customWidth="1"/>
-    <col min="3" max="3" width="63.796875" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+    <col min="3" max="3" width="63.77734375" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="40.1328125" customWidth="1"/>
-    <col min="6" max="6" width="12.86328125" customWidth="1"/>
+    <col min="5" max="5" width="40.109375" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" customWidth="1"/>
     <col min="7" max="7" width="54.33203125" customWidth="1"/>
-    <col min="9" max="9" width="23.19921875" customWidth="1"/>
+    <col min="9" max="9" width="23.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1208,7 +1209,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>